<commit_message>
Updated citations; formatted for PLoS ONE; moved textbox in methods (not allowed); removed supplemntal table 2 (not updated; too late to fix)
git-svn-id: http://svn.code.sf.net/p/obi/code@4024 a3e8fd31-a726-0410-8195-c3f0c8a19530
</commit_message>
<xml_diff>
--- a/trunk/docs/papers/release/2015 PLoS ONE submission/Supplemental Table 1.xlsx
+++ b/trunk/docs/papers/release/2015 PLoS ONE submission/Supplemental Table 1.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bpeters\Documents\obi\docs\papers\release\2015 PLoS ONE submission\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="96" windowWidth="22992" windowHeight="11568"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="22995" windowHeight="11565"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>Project Name</t>
   </si>
@@ -196,9 +191,6 @@
     <t>BioSharing</t>
   </si>
   <si>
-    <t>BioSharing is a web-based, curated and searchable portal ensuring that standards, databases and policies in the life sciences are registered, informative and discoverable. BioSharing is also part of the ELIXIR UK node interoperability components of the EXCELERATE project (http://elixir-uk.org/interoperability-infrastructure).</t>
-  </si>
-  <si>
     <t>BioSharing uses OBI as a source of controlled terms.</t>
   </si>
   <si>
@@ -406,17 +398,10 @@
     <t>CogPO is a framework for the formal representation of the cognitive paradigms used in behavioral experiments, driven by cognitive neuroscience and neuroimaging examples.</t>
   </si>
   <si>
-    <t>The ISA (Investigation/Study/Assay) infrastructure is a user-friendly multi-domain data capture and management suite that allows the searching of OBI for terms to use in data entry. The ISA infrastructure is also part of the ELIXIR UK node interoperability components of the EXCELERATE project (http://elixir-uk.org/interoperability-infrastructure).</t>
-  </si>
-  <si>
     <t>AERO is an ontology aimed at supporting clinicians at the time of data entry, increasing quality and accuracy of reported adverse events.</t>
   </si>
   <si>
     <t>STATO is a general-purpose STATistics Ontology. Its aim is to provide coverage for processes such as statistical tests, their conditions of application, and information needed or resulting from statistical methods, such as probability distributions, variables, spread and variation metrics. STATO also covers aspects of experimental design and description of plots and graphical representations commonly used to provide visual cues of data distribution or layout and to assist review of the results.</t>
-  </si>
-  <si>
-    <t>OntoDM-core defines the most essential data mining entities in a three-layered ontological structure comprising of a specification, an implementation and an application layer. It provides a representational framework for the description of mining structured data, and in addition provides taxonomies of datasets, data mining tasks, generalizations, 
-data mining algorithms and constraints, based on the type of data.</t>
   </si>
   <si>
     <t>The Ontology of Biological and Clinical Statistics (OBCS) is a biomedical ontology in the domain of biological and clinical statistics. OBCS is primarily targeted for statistical term representation in the fields in biological, biomedical, and clinical domains.</t>
@@ -448,6 +433,69 @@
   </si>
   <si>
     <t>OBI is used as a middle-layer ontology providing relations and terms needed to denote the diagnosis process performed by medical experts when analyzing adverse event reports.</t>
+  </si>
+  <si>
+    <t>The ISA (Investigation/Study/Assay) infrastructure is a user-friendly multi-domain data capture and management suite that allows the searching of OBI for terms to use in data entry. The ISA infrastructure is also part of the ELIXIR UK node interoperability components of the EXCELERATE project.</t>
+  </si>
+  <si>
+    <t>BioSharing is a web-based, curated and searchable portal ensuring that standards, databases and policies in the life sciences are registered, informative and discoverable. BioSharing is also part of the ELIXIR UK node interoperability components of the EXCELERATE project.</t>
+  </si>
+  <si>
+    <t>OntoDM-core defines the most essential data mining entities in a three-layered ontological structure comprising of a specification, an implementation and an application layer. It provides a representational framework for the description of mining structured data, and in addition provides taxonomies of datasets, data mining tasks, generalizations, data mining algorithms and constraints, based on the type of data.</t>
+  </si>
+  <si>
+    <t>RRID:nlx_157524</t>
+  </si>
+  <si>
+    <t>miRNA and Aging Ontology (MIAGO)</t>
+  </si>
+  <si>
+    <t>The miRNA and aging ontology (MIAGO) represents miRNA, miRNA targets, experimental assays, miRNA target assumption, and miRNA target evidence. MIAGO establishes an OWL-based descriptive logic reasoning approach to measure the validation level of miRNA and target assumption by combining different kinds of experimental evidence and computational prediction.</t>
+  </si>
+  <si>
+    <t>MIAGO is built on top of OBI and BFO, with OBI's assay model as the core component of MIAGO. MIAGO defines the conclusion of an assay as evidence and then links that evidence back to different assays.</t>
+  </si>
+  <si>
+    <t>https://github.com/linikujp/miraging</t>
+  </si>
+  <si>
+    <t>Informed Consent Ontology (ICO)</t>
+  </si>
+  <si>
+    <t>The Informed Consent Ontology (ICO) represents the documentations and processes involved in informed consent. ICO aims to support informed consent data integration and reasoning in the clinical research space.</t>
+  </si>
+  <si>
+    <t>ICO imports BFO, OBI and IAO. ICO extends the OBI term 'informed consent process' by introducing the informed consent specific processes.</t>
+  </si>
+  <si>
+    <t>https://github.com/ICO-ontology/ICO</t>
+  </si>
+  <si>
+    <t>Vaccination Informed Consent Ontology (VICO)</t>
+  </si>
+  <si>
+    <t>The Vaccination Informed Consent Ontology (VICO) represents entities related to vaccination specfic informed consents with a special focus on vaccination informed consent forms, contents, and questionnaires in the forms.</t>
+  </si>
+  <si>
+    <t>VICO extends Informed Consent Ontology (ICO) and integrates Vaccine Ontology (VO). Both ICO and VO are BFO and OBI based ontologies, which makes VICO a BFO and OBI based ontology as well.</t>
+  </si>
+  <si>
+    <t>https://github.com/VICO-ontology/VICO</t>
+  </si>
+  <si>
+    <t>Brucellosis Ontology (IDOBRU)</t>
+  </si>
+  <si>
+    <t>IDOBRU ontologically represents different aspects of brucellosis, including the host infection, zoonotic disease transmission, symptoms, virulence factors and pathogenesis, diagnosis, intentional release, vaccine prevention, and treatment.</t>
+  </si>
+  <si>
+    <t>IDOBRU is aligned with and imports 21 terms from OBI, e.g., organism, PRC, specimen, specimen role, and planned process.</t>
+  </si>
+  <si>
+    <t>http://www.ontobee.org/ontology/IDOBRU</t>
+  </si>
+  <si>
+    <t>RRID:nlx_157345</t>
   </si>
 </sst>
 </file>
@@ -484,18 +532,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -507,17 +549,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,16 +568,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,26 +580,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -626,7 +644,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -661,7 +679,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -873,22 +891,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="38" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="48.44140625" customWidth="1"/>
-    <col min="4" max="4" width="42.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -896,514 +914,585 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E11" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="12" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C18" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="D22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="117.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E25" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="26" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E30" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="66" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="66" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="4" t="s">
+    <row r="31" spans="1:5" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="66" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E31" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="7" t="s">
+    <row r="32" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C33" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="E33" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="79.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="66" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" s="8"/>
     </row>
   </sheetData>
+  <sortState ref="A2:E33">
+    <sortCondition ref="A1"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2" display="http://iedb.org/"/>
-    <hyperlink ref="D4" r:id="rId3" display="http://www.neuinfo.org/"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D18" r:id="rId2" display="http://iedb.org/"/>
+    <hyperlink ref="D25" r:id="rId3" display="http://www.neuinfo.org/"/>
+    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="D30" r:id="rId5"/>
+    <hyperlink ref="D26" r:id="rId6"/>
+    <hyperlink ref="D5" r:id="rId7"/>
+    <hyperlink ref="D17" r:id="rId8"/>
+    <hyperlink ref="D19" r:id="rId9"/>
+    <hyperlink ref="D14" r:id="rId10"/>
     <hyperlink ref="D12" r:id="rId11" display="http://www.eagle-i.net/"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13" display="http://www.biosharing.org/"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15" display="http://www.cvrgrid.org/"/>
-    <hyperlink ref="D17" r:id="rId16"/>
-    <hyperlink ref="D18" r:id="rId17"/>
-    <hyperlink ref="D19" r:id="rId18"/>
-    <hyperlink ref="D20" r:id="rId19"/>
-    <hyperlink ref="D21" r:id="rId20"/>
-    <hyperlink ref="D22" r:id="rId21" display="http://www.evidenceontology.org/"/>
-    <hyperlink ref="D23" r:id="rId22"/>
-    <hyperlink ref="D24" r:id="rId23" display="http://stato-ontology.org/"/>
-    <hyperlink ref="D25" r:id="rId24"/>
-    <hyperlink ref="D26" r:id="rId25" display="http://www.nano-ontology.org/"/>
-    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D31" r:id="rId12"/>
+    <hyperlink ref="D6" r:id="rId13" display="http://www.biosharing.org/"/>
+    <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="D8" r:id="rId15" display="http://www.cvrgrid.org/"/>
+    <hyperlink ref="D23" r:id="rId16"/>
+    <hyperlink ref="D24" r:id="rId17"/>
+    <hyperlink ref="D3" r:id="rId18"/>
+    <hyperlink ref="D2" r:id="rId19"/>
+    <hyperlink ref="D33" r:id="rId20"/>
+    <hyperlink ref="D15" r:id="rId21" display="http://www.evidenceontology.org/"/>
+    <hyperlink ref="D9" r:id="rId22"/>
+    <hyperlink ref="D29" r:id="rId23" display="http://stato-ontology.org/"/>
+    <hyperlink ref="D13" r:id="rId24"/>
+    <hyperlink ref="D22" r:id="rId25" display="http://www.nano-ontology.org/"/>
+    <hyperlink ref="D10" r:id="rId26"/>
     <hyperlink ref="D28" r:id="rId27" display="http://www.ontodm.com/"/>
-    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D27" r:id="rId28"/>
+    <hyperlink ref="D21" r:id="rId29"/>
+    <hyperlink ref="D20" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D7" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="31" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId29"/>
+  <pageSetup scale="31" orientation="landscape" horizontalDpi="4294967293" r:id="rId33"/>
 </worksheet>
 </file>
 
@@ -1413,7 +1502,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1425,7 +1514,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>